<commit_message>
accumulator still had value in it
</commit_message>
<xml_diff>
--- a/GCSE/resources/fetch-decode-execute.xlsx
+++ b/GCSE/resources/fetch-decode-execute.xlsx
@@ -1340,7 +1340,7 @@
   <dimension ref="B1:U21"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="R14" sqref="R14"/>
+      <selection activeCell="C5" sqref="C5:E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1397,9 +1397,7 @@
     </row>
     <row r="5" spans="2:21" x14ac:dyDescent="0.35">
       <c r="B5" s="10"/>
-      <c r="C5" s="33">
-        <v>20</v>
-      </c>
+      <c r="C5" s="33"/>
       <c r="D5" s="33"/>
       <c r="E5" s="33"/>
       <c r="F5" s="1"/>

</xml_diff>